<commit_message>
Updated and frozen InventoryProxy requirements
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.001.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.001.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\subscripton\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\affaince\documentation\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Terminologies used" sheetId="7" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="171">
   <si>
     <t>Domains</t>
   </si>
@@ -278,13 +278,7 @@
     <t>As an Administrator I will retrieve the list of available items from current inventory of shopping application by providing category and subcategory as a search criteria so as to register them to be subcriptionable item.</t>
   </si>
   <si>
-    <t>Need to discuss</t>
-  </si>
-  <si>
     <t>Periodic batch operations</t>
-  </si>
-  <si>
-    <t>As a system I will generate a file on a daily basis containing the subscriberId,category id,subcategory Id,item id,quoted price each item subscribed under his basket for which the delivery of respective basekts was due on that day so as to make the dispatch application verify the same against the deliveries that they have made on that day.</t>
   </si>
   <si>
     <t>As an Administrator  I will fill a  CSV file having the following attributes
@@ -294,34 +288,7 @@
 and uploads it in the system so as to make these items available for registration for subscription.</t>
   </si>
   <si>
-    <t>As a system I will retrieve the Category(CategoryId,Category Name), subcategory(subcategory id and subcategory name),Item under each category/subcategory only those which are registered as subscriptionable item,its current purchase price,its current stock and its current MRP on a daily basis so as to maintain/update the inventory proxy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a system I will generate a file containing the subscriptionable item with its category id,subcategory id,total registerd volume of subscriptions in a day, for it,quoted subcription price per unit,derived sale price per unit after including additional discounts/offers(if any) at the end of the day for it to be consumed by the main application inventory for their update purpose. </t>
-  </si>
-  <si>
-    <t>Daily retrival of subscriptionable items datails from main store</t>
-  </si>
-  <si>
-    <t>Generate new subscriptions details on day</t>
-  </si>
-  <si>
-    <t>Notify Dispatch on the deliveries on a day</t>
-  </si>
-  <si>
-    <t>System will receive the status of raised dispatch requests,from dispatch/delivery departments so as to update the same in the repository and it processes it .</t>
-  </si>
-  <si>
     <t>Update status of targeted dispatches on every day</t>
-  </si>
-  <si>
-    <t>System will generate an End of Day report of the incomplete dispatches and the reasons for the same containing subscription baskeet Id (which is same as Subscriber Id),Subscription items targetted for dispatch and the reason code for inability to dispatch items.</t>
-  </si>
-  <si>
-    <t>Generate a report of undispatched baskets</t>
-  </si>
-  <si>
-    <t>As a system I will generate dispatch requests for the deliveries to be made on a day to be sent to dispatch department</t>
   </si>
   <si>
     <t>Mass upload of item configuration</t>
@@ -600,12 +567,39 @@
 5. Unit (currency or days)
 There can be multiple eligibility criterias. In that case, I as administrator will add those by selecting above 5 parameters for each criteria.</t>
   </si>
+  <si>
+    <t>Epic</t>
+  </si>
+  <si>
+    <t>Generate dispatch requests for the next day</t>
+  </si>
+  <si>
+    <t>As a system I will generate a file on a daily basis containing the subscriberId,list of products selected by him/her(category id,subcategory Id,item id,quoted price of each item subscribed under his basket) and intended delivery date  so as to make the dispatch department enable the actual dispatch of these items as well as consolidate if the required dispatch were made on that day or not.</t>
+  </si>
+  <si>
+    <t>System will receive the status(DISPATCH,DEIVERED,DELIVERY FAILED) with reason code  of raised dispatch requests,from dispatch/delivery departments in the form of a flat file so as to update the same in the repository .</t>
+  </si>
+  <si>
+    <t>Daily retrival of subscriptionable items datails from main store.</t>
+  </si>
+  <si>
+    <t>During transition of one batch of product to new batch the purchase price may change.</t>
+  </si>
+  <si>
+    <t>As a system I will retrieve the BatchID,Category(CategoryId,Category Name), subcategory(subcategory id and subcategory name),Item under each category/subcategory only those which are registered as subscriptionable item,its latest purchase price,its current stock,its current MRP and its current quoted price(for instantanious sale) on a daily basis so as to maintain/update the inventory proxy.</t>
+  </si>
+  <si>
+    <t>Should I forecast for the probable increase of demand in the remaining days of month.</t>
+  </si>
+  <si>
+    <t>As a system I will generate a flat file containing category,subcategory, subscriptionable item id and its current stock requirement (as of the day) and increment in the stock as compared to earlier day which can be considered as a forecast of next three months for the inventory department.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -617,6 +611,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -657,7 +657,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -682,6 +682,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -979,66 +982,66 @@
   <sheetData>
     <row r="2" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C2" s="7" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C6" s="6" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C7" s="6" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="6" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C9" s="6" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.25">
@@ -2577,267 +2580,256 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B24" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="47.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="47.7109375" style="3"/>
-    <col min="2" max="2" width="57.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.42578125" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="47.7109375" style="3"/>
+    <col min="1" max="2" width="47.7109375" style="3"/>
+    <col min="3" max="3" width="57.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.42578125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="47.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="4"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="150" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="C13" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" s="3" t="s">
+      <c r="B14" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="180" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
-        <v>99</v>
-      </c>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="C21" s="5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="225" x14ac:dyDescent="0.25">
-      <c r="B22" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="165" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+      <c r="C22" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="C23" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="C24" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="C26" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="D27" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+      <c r="C28" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="D29" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="C30" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="D31" s="8" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="C32" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="165" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="135" x14ac:dyDescent="0.25">
-      <c r="C27" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="180" x14ac:dyDescent="0.25">
-      <c r="B28" s="3" t="s">
-        <v>166</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="135" x14ac:dyDescent="0.25">
-      <c r="C29" s="8" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="165" x14ac:dyDescent="0.25">
-      <c r="B30" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="135" x14ac:dyDescent="0.25">
-      <c r="C31" s="8" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="165" x14ac:dyDescent="0.25">
-      <c r="B32" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="33" spans="3:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="C33" s="8" t="s">
-        <v>170</v>
+    <row r="33" spans="4:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="D33" s="8" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2847,18 +2839,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I87"/>
+  <dimension ref="A2:I83"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" style="3" customWidth="1"/>
-    <col min="2" max="2" width="69.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="79" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="4" max="4" width="79.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2885,62 +2878,57 @@
     </row>
     <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>88</v>
+        <v>166</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>87</v>
+        <v>135</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>170</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>82</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>89</v>
+        <v>163</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
@@ -2949,7 +2937,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
+      <c r="B11" s="2"/>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2958,27 +2946,19 @@
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
-        <v>27</v>
-      </c>
+      <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
@@ -2998,7 +2978,6 @@
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
@@ -3018,6 +2997,7 @@
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
@@ -3051,22 +3031,18 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
       <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
       <c r="C33" s="1"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -3079,18 +3055,22 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
+      <c r="B37" s="2"/>
       <c r="C37" s="1"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
+      <c r="B38" s="2"/>
       <c r="C38" s="1"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -3100,12 +3080,12 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-      <c r="B41" s="2"/>
+      <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-      <c r="B42" s="2"/>
+      <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -3125,17 +3105,17 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
+      <c r="B46" s="2"/>
       <c r="C46" s="1"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
+      <c r="B47" s="2"/>
       <c r="C47" s="1"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
+      <c r="B48" s="2"/>
       <c r="C48" s="1"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
@@ -3145,12 +3125,12 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="B50" s="2"/>
+      <c r="B50" s="1"/>
       <c r="C50" s="1"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
-      <c r="B51" s="2"/>
+      <c r="B51" s="1"/>
       <c r="C51" s="1"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -3175,7 +3155,7 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
-      <c r="B56" s="2"/>
+      <c r="B56" s="1"/>
       <c r="C56" s="1"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
@@ -3312,26 +3292,6 @@
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="1"/>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3341,10 +3301,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3374,310 +3334,406 @@
       <c r="I1" s="4"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>29</v>
-      </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
-        <v>153</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>154</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
-        <v>148</v>
-      </c>
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
-      <c r="C7" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
-        <v>152</v>
-      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="3" t="s">
-        <v>149</v>
-      </c>
+      <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>31</v>
-      </c>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C17" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="C19" s="1" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="C20" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>142</v>
+      </c>
       <c r="C21" s="1" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
+      <c r="B23" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="C23" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
+      <c r="B26" s="3" t="s">
+        <v>138</v>
+      </c>
       <c r="C26" s="1" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="C27" s="1"/>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="1"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="1"/>
-    </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-      <c r="B34" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C34" s="1"/>
-    </row>
-    <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C35" s="1"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-    </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C38" s="1"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="C38" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="1"/>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="1"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-    </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C42" s="1"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="C42" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-      <c r="B43" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C43" s="1"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
-      <c r="B44" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="1"/>
+    </row>
+    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C49" s="1"/>
+    </row>
+    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C50" s="1"/>
+    </row>
+    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C51" s="1"/>
+    </row>
+    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52" s="1"/>
+      <c r="B52" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C52" s="1"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1"/>
+      <c r="B53" s="1"/>
+      <c r="C53" s="1"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="1"/>
+      <c r="C54" s="1"/>
+    </row>
+    <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55" s="1"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="2"/>
+      <c r="C56" s="1"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="1"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+    </row>
+    <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59" s="1"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60" s="1"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1"/>
+      <c r="B61" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61" s="1"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1"/>
+      <c r="B62" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="1"/>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
+      <c r="C62" s="1"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1"/>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1"/>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3869,18 +3925,18 @@
     </row>
     <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="C3" s="8" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified requirements related to ItemSubscription
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.001.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.001.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Terminologies used" sheetId="7" r:id="rId1"/>
     <sheet name="Summary" sheetId="1" r:id="rId2"/>
-    <sheet name="Configuration" sheetId="6" r:id="rId3"/>
+    <sheet name="ItemSubscription" sheetId="6" r:id="rId3"/>
     <sheet name="InventoryProxy" sheetId="2" r:id="rId4"/>
     <sheet name="UserSubscription" sheetId="3" r:id="rId5"/>
     <sheet name="PricingEngine" sheetId="4" r:id="rId6"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="181">
   <si>
     <t>Domains</t>
   </si>
@@ -264,9 +264,6 @@
   </si>
   <si>
     <t>As an administrator I will configure the minimum thrshold amount of the basket for which the basket may be elligible for baset level discount.</t>
-  </si>
-  <si>
-    <t>May need to move it to offers &amp; rewards</t>
   </si>
   <si>
     <t>System will validate the received category information and Item information against the main application inventory as well as retrieve additional information such as category/sbcategory name,item name,manufacturer Id and Name,purchase price,MRP,current stock so as to list them on Configuration UI for the registration purpose.</t>
@@ -289,9 +286,6 @@
   </si>
   <si>
     <t>Update status of targeted dispatches on every day</t>
-  </si>
-  <si>
-    <t>Mass upload of item configuration</t>
   </si>
   <si>
     <t>As an administrator I will configure the rule for the subscription basket such that maximum permissible subscription period of any item in the basket should not exceed configured duration as number and unit(month, year).</t>
@@ -396,9 +390,6 @@
     <t>As an administrator I can configure the maximum number of subscription baskets a subscriber can have.</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
     <t xml:space="preserve">As a User  I add a subscription item to a subscription basket by providing qunatity per cycle, so as to subscribe for that item.   </t>
   </si>
   <si>
@@ -494,21 +485,6 @@
   </si>
   <si>
     <t>As a system I may ask registerd user to provide one time registration charges to be paid by him/her to register as a subscriber.</t>
-  </si>
-  <si>
-    <t>Discount based on Subscription Basket</t>
-  </si>
-  <si>
-    <t>Create offer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a administrator I will configure eligibility  criterias Total Amount and Subscription period by setting parameters comparator (less that equal to, greater than equal to), value type (time period, amount), value and unit (currency, days) as to create offer. </t>
-  </si>
-  <si>
-    <t>As a administrator I will configure benefit type (Amount, percentage, cashback, material) by setting parameters  benefit, unit of benefit (currency, percentage), time period for cashback and material type as to create offer.</t>
-  </si>
-  <si>
-    <t>Create Offer Strategies</t>
   </si>
   <si>
     <t>Create offer based on Subscription basket</t>
@@ -568,9 +544,6 @@
 There can be multiple eligibility criterias. In that case, I as administrator will add those by selecting above 5 parameters for each criteria.</t>
   </si>
   <si>
-    <t>Epic</t>
-  </si>
-  <si>
     <t>Generate dispatch requests for the next day</t>
   </si>
   <si>
@@ -593,6 +566,63 @@
   </si>
   <si>
     <t>As a system I will generate a flat file containing category,subcategory, subscriptionable item id and its current stock requirement (as of the day) and increment in the stock as compared to earlier day which can be considered as a forecast of next three months for the inventory department.</t>
+  </si>
+  <si>
+    <t>As an Administrator I will retrieve the list of available items from current inventory of shopping application,optionally by providing category and subcategory as a search criteria so as to register them to be subcriptionable item.</t>
+  </si>
+  <si>
+    <t>As an administrator I will select an item to be register as a subscriptionable item and register it with system so that only these items will be available for periodic subscriptions.</t>
+  </si>
+  <si>
+    <t>As an administrator I will update Target consumption period(monthly,quarterly,half yearly,yearly), target sale quantity(example: 5000 units per quarter etc) per consumption period, minimum profit margin(percentage), maximum profit margin, Demand to supply ratio, consumption frequency(units per month)  for the registered item to register it as a subscriptionable item.</t>
+  </si>
+  <si>
+    <t>As a administrator I will "add" a new configuration paramter as Target Consumption period and its value with unit(1 month,1 yearetc)</t>
+  </si>
+  <si>
+    <t>As an administrator I will "add" a new configuration paramter "target sale per consumption period"and its value and unit.</t>
+  </si>
+  <si>
+    <t>As an administrator I will "add" a new configuration paramter "minimum profit margin", its value and unit.</t>
+  </si>
+  <si>
+    <t>As an administrator I will "add" a  new configuration parameter "maximum profit margin",its value and unit.</t>
+  </si>
+  <si>
+    <t>As an administrator I will "add" a  new configuration parameter "demand to supply ratio",its value and unit.</t>
+  </si>
+  <si>
+    <t>As an administrator I will "add" a  new configuration parameter "consumption frequency",its value and unit.</t>
+  </si>
+  <si>
+    <t>Mass upload</t>
+  </si>
+  <si>
+    <t>As an administrator I can add a new subscription rule "minimum permissible discount",its value and unit for a subscriptionable item so that subscriber fitting into various offers criterias can get minimum this vaue as discount.</t>
+  </si>
+  <si>
+    <t>As an administrator I can define the maximum discount percentage permissible for a subscriptionable item(including the added discounts due to offers and rewards).</t>
+  </si>
+  <si>
+    <t>As an administrator I can add a new subscription rule "maximum permissible discount",its value and unit for a subscriptionable item so that subscriber fitting into various offers criterias can get upto this value as discount.</t>
+  </si>
+  <si>
+    <t>As an administrator I can define maximum units of a subscriptionable itemthose can be subscribed per subscription cycle</t>
+  </si>
+  <si>
+    <t>As an administrator I can add a new subscription rule "maximum permissible units",its value and unit for a subscriptionable item so that subscriber can order upto this value per subscripton cycle.</t>
+  </si>
+  <si>
+    <t>As an administrator I will add new rule  "maximum permissible subscription period ",it value and unit so that any item cannot be subscribed at a time for more than the given value.</t>
+  </si>
+  <si>
+    <t>As an administrator I will add a new rule for the subscription basket "maximum permissible amount of the basket", as value and unit(rupees,dollor,euro etc)</t>
+  </si>
+  <si>
+    <t>As an administrator I will add a new rule "minimum threshold amount of basket for discount eligiibiity", value and unit for which the basket may be elligible for basket level discount/offer.</t>
+  </si>
+  <si>
+    <t>As an administrator I will add a new rule "maximum permissible discount", unit and value so that any subscriber cannot get discount more than the one defined here .</t>
   </si>
 </sst>
 </file>
@@ -982,66 +1012,66 @@
   <sheetData>
     <row r="2" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C2" s="7" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C6" s="6" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C7" s="6" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="6" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C9" s="6" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.25">
@@ -2580,11 +2610,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:D18"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="47.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2599,238 +2627,251 @@
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+    </row>
+    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="5" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="D8" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="1"/>
+      <c r="D9" s="5" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="1"/>
+      <c r="D10" s="5" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="1"/>
+      <c r="D11" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>134</v>
+        <v>171</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="1" t="s">
-        <v>116</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>78</v>
-      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>129</v>
+      </c>
       <c r="B15" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:10" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="C19" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+      <c r="B25" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D25" s="5"/>
+    </row>
+    <row r="26" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="180" x14ac:dyDescent="0.25">
-      <c r="C21" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" s="5" t="s">
+      <c r="C26" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="225" x14ac:dyDescent="0.25">
-      <c r="C22" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D22" s="5" t="s">
+      <c r="C27" s="5" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="C23" s="3" t="s">
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="C28" s="5" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="150" x14ac:dyDescent="0.25">
-      <c r="C24" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="C26" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="D27" s="8" t="s">
-        <v>159</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="180" x14ac:dyDescent="0.25">
-      <c r="C28" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="D29" s="8" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="C30" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="135" x14ac:dyDescent="0.25">
-      <c r="D31" s="8" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="165" x14ac:dyDescent="0.25">
-      <c r="C32" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4" ht="135" x14ac:dyDescent="0.25">
-      <c r="D33" s="8" t="s">
-        <v>159</v>
-      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2841,7 +2882,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -2878,46 +2919,46 @@
     </row>
     <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3342,19 +3383,19 @@
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3362,26 +3403,26 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3389,12 +3430,12 @@
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -3406,13 +3447,13 @@
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -3420,13 +3461,13 @@
         <v>17</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3440,52 +3481,52 @@
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3497,54 +3538,54 @@
         <v>31</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3562,31 +3603,31 @@
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -3598,7 +3639,7 @@
     <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="C43" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3899,20 +3940,21 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.7109375" customWidth="1"/>
     <col min="3" max="3" width="97.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -3923,21 +3965,71 @@
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="B2" t="s">
-        <v>147</v>
+    <row r="2" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>143</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="B3" s="3"/>
       <c r="C3" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+      <c r="C5" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
         <v>149</v>
       </c>
+      <c r="C6" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
+      <c r="C7" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
+      <c r="C9" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated requirements for Offers and Discounts
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.001.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.001.xlsx
@@ -9,16 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Terminologies used" sheetId="7" r:id="rId1"/>
-    <sheet name="Summary" sheetId="1" r:id="rId2"/>
-    <sheet name="ItemSubscription" sheetId="6" r:id="rId3"/>
-    <sheet name="InventoryProxy" sheetId="2" r:id="rId4"/>
-    <sheet name="UserSubscription" sheetId="3" r:id="rId5"/>
-    <sheet name="PricingEngine" sheetId="4" r:id="rId6"/>
-    <sheet name="Offers And Rewards" sheetId="5" r:id="rId7"/>
+    <sheet name="ItemSubscription" sheetId="6" r:id="rId2"/>
+    <sheet name="InventoryProxy" sheetId="2" r:id="rId3"/>
+    <sheet name="UserSubscription" sheetId="3" r:id="rId4"/>
+    <sheet name="PricingEngine" sheetId="4" r:id="rId5"/>
+    <sheet name="Offers And Rewards" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,95 +29,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="181">
-  <si>
-    <t>Domains</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="144">
   <si>
     <t>Epics</t>
   </si>
   <si>
-    <t>User stories</t>
-  </si>
-  <si>
-    <t>InventoryProxy</t>
-  </si>
-  <si>
     <t>Item Registration</t>
   </si>
   <si>
     <t>Register a subscriptionable item(for making it available for subscriptions by customers</t>
   </si>
   <si>
-    <t>As an administrator I will retrieve the Category(CategoryId,Category Name) and subcategory(subcategory id and subcategory name) of products so as to maintain them in the inventory proxy.</t>
-  </si>
-  <si>
-    <t>As a Administrator I will retrieve the list of available items from current inventory of shopping application so as to register them to be subcriptionable item.</t>
-  </si>
-  <si>
-    <t>As an administrator I will update Target cosumtpion period(monthly,quarterly,half yearly,yearly), target sale quantity(example: 5000 units per quarter etc).,minimum profit margin(percentage),maximum profit margin,Demand density(very high,high,medium,low,very low),Demand to supply ratio,consumption frequency(high,low,medium)  for the rerieved item to register as a subscriptionable item</t>
-  </si>
-  <si>
-    <t>Sytstem generates categorywise report of the items registered as subscriptionable item against the list of all items being sold by the parent shopping application so as to verify if any item is left to be registered as subscriptionable item.</t>
-  </si>
-  <si>
-    <t>As an administratorI will configure the rules for the subscription baskets such as maximum permissible amount of the basket,as number and unit(rupees,dollor,euro etc)</t>
-  </si>
-  <si>
-    <t>Basket configuration</t>
-  </si>
-  <si>
     <t>Configure rules for subscription basket</t>
   </si>
   <si>
-    <t>As an administrator I will cnfigure the rule for the subscription basket such that aximum permissible subscription period of any item in the basket should not exceed one year.</t>
-  </si>
-  <si>
-    <t>As an administrator I will configure the minimum thrshold amount of the basket for which minimum category of additional discount will be applied.</t>
-  </si>
-  <si>
-    <t>As an administrator I will configure the average thrshold amount of the basket for which average category of additional discount will be applied.</t>
-  </si>
-  <si>
-    <t>As an administrator I will configure the maximum thrshold amount of the basket for which maximum category of additional discount will be applied.</t>
-  </si>
-  <si>
     <t>Mass upload of subscriptionable item definitions</t>
   </si>
   <si>
-    <t>Notifications</t>
-  </si>
-  <si>
-    <t>Receive current stock of each subscriptionable item from main store</t>
-  </si>
-  <si>
-    <t>Receive notification from notification domain to deliver a subscriptionable item to a user</t>
-  </si>
-  <si>
-    <t>Packging</t>
-  </si>
-  <si>
-    <t>Package different subscriptionable tems to be delivered to a single subcriber</t>
-  </si>
-  <si>
-    <t>Dispatch package to a subscriber</t>
-  </si>
-  <si>
-    <t>Update inventory after dispatching list of items to a subscriber</t>
-  </si>
-  <si>
-    <t>Analytics</t>
-  </si>
-  <si>
-    <t>Calculate total demand per subscriptionable item</t>
-  </si>
-  <si>
-    <t>Generate item wise supply vs demand report on a daily basis</t>
-  </si>
-  <si>
-    <t>Subscripton</t>
-  </si>
-  <si>
     <t>User subscription</t>
   </si>
   <si>
@@ -128,57 +55,18 @@
     <t>A subscriber subscribing to a subscriptionable item</t>
   </si>
   <si>
-    <t xml:space="preserve">As a User  I subscribe to a subscription item by providing qunatity per cycle, subscription cycle in the form of  Number describing periodicity , and unit for it( 2 week,3 month etc.) so as to subscribe for that item.   </t>
-  </si>
-  <si>
     <t>System receiving price quote for the subscibed item on the day of subscription from Pricing domain</t>
   </si>
   <si>
-    <t>System receives current price quote for the the subscription item which the user is intending to subscribe and show it as today's price,MRP, perentage gain.</t>
-  </si>
-  <si>
-    <t>As a User I keep on adding subscription items so as to build my subscription basket and finally checkout the basket after finalizing subscription items so as to get the total price to be paid as well as total gain( as compared to total MRP).</t>
-  </si>
-  <si>
-    <t>System will offer me PrePaid payment mode where I will pay for the whole amount for the selected subscription period in advance.</t>
-  </si>
-  <si>
-    <t>System will offer me the PostPaid payment mode where I will make payment on delivery for each subcripton cycle.</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>System will offer me the PartialPaid payment mode so that I can pay 30% of the total amount to be paid for the whole subscription period.</t>
-  </si>
-  <si>
-    <t>As a user I will select the payment mode out of following payment modes( Prepaid,Postpaid,PartialPaid) so as to account the discount associated with payment mode.</t>
-  </si>
-  <si>
-    <t>System will calculate the additional discount per basket if any, only if the minimum threshold amount for the basket is overcome.</t>
-  </si>
-  <si>
-    <t>System displays subscription basket containing list of intended subscription items'  total payable price per item,total MRP per item, total amout to be paid for the basket ,total MRP for the basket  and total savings in percentage  and in amount per basket per cycle.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a User I enter billing address,delivery address,so as to receive items package and bill.  </t>
-  </si>
-  <si>
     <t>System retrieves other user information like e-mail address and phone number from main application and attach to subscription basket.</t>
   </si>
   <si>
     <t>As a user I can add a new subcrptionable item to my subcription basket from the subcription basket screen.</t>
   </si>
   <si>
-    <t>As a user  can modify the quantity or subcription cycle of one or many subcriptionable items from subscription baskeet screen</t>
-  </si>
-  <si>
     <t>As a user I can delete an already subscribed subscriptionable item from subscription basket screen.</t>
   </si>
   <si>
-    <t>In case of addition/modification/deletion of subscriptionable items from the basket or in case of change of payment mode,system will recalculate the total payable amount as well as totoal discounts.</t>
-  </si>
-  <si>
     <t>Subscriber makes payment for the periodic subscription of subscriptionable items(different payment schemes?)</t>
   </si>
   <si>
@@ -224,9 +112,6 @@
     <t>System recovers maximum pending pament form the available deposit.</t>
   </si>
   <si>
-    <t>Pricing</t>
-  </si>
-  <si>
     <t>Configure system for the price calculation options.</t>
   </si>
   <si>
@@ -252,9 +137,6 @@
   </si>
   <si>
     <t>Pricing Model2</t>
-  </si>
-  <si>
-    <t>Integration</t>
   </si>
   <si>
     <t>User Stories</t>
@@ -502,127 +384,148 @@
     <t>Create offer based on Brand Loyalty</t>
   </si>
   <si>
-    <t>As a administrator I will create new offer strategy where I will choose offer type as "Discount based on Subscription basket" and selects the following
-1. Eligibility  criteria (Total Amount or Subscription period)
-2. Comparator (less that equal to or greater than equal to)
-3. Value type (time period or amount)
-4. Value
-5. Unit (currency or days)
-There can be multiple eligibility criterias. In that case, I as administrator will add those by selecting above 5 parameters for each criteria.</t>
-  </si>
-  <si>
     <t>Create offer based on Customer Loyalty</t>
+  </si>
+  <si>
+    <t>Create surprise offer</t>
+  </si>
+  <si>
+    <t>Generate dispatch requests for the next day</t>
+  </si>
+  <si>
+    <t>As a system I will generate a file on a daily basis containing the subscriberId,list of products selected by him/her(category id,subcategory Id,item id,quoted price of each item subscribed under his basket) and intended delivery date  so as to make the dispatch department enable the actual dispatch of these items as well as consolidate if the required dispatch were made on that day or not.</t>
+  </si>
+  <si>
+    <t>System will receive the status(DISPATCH,DEIVERED,DELIVERY FAILED) with reason code  of raised dispatch requests,from dispatch/delivery departments in the form of a flat file so as to update the same in the repository .</t>
+  </si>
+  <si>
+    <t>Daily retrival of subscriptionable items datails from main store.</t>
+  </si>
+  <si>
+    <t>During transition of one batch of product to new batch the purchase price may change.</t>
+  </si>
+  <si>
+    <t>As a system I will retrieve the BatchID,Category(CategoryId,Category Name), subcategory(subcategory id and subcategory name),Item under each category/subcategory only those which are registered as subscriptionable item,its latest purchase price,its current stock,its current MRP and its current quoted price(for instantanious sale) on a daily basis so as to maintain/update the inventory proxy.</t>
+  </si>
+  <si>
+    <t>Should I forecast for the probable increase of demand in the remaining days of month.</t>
+  </si>
+  <si>
+    <t>As a system I will generate a flat file containing category,subcategory, subscriptionable item id and its current stock requirement (as of the day) and increment in the stock as compared to earlier day which can be considered as a forecast of next three months for the inventory department.</t>
+  </si>
+  <si>
+    <t>As an Administrator I will retrieve the list of available items from current inventory of shopping application,optionally by providing category and subcategory as a search criteria so as to register them to be subcriptionable item.</t>
+  </si>
+  <si>
+    <t>As an administrator I will select an item to be register as a subscriptionable item and register it with system so that only these items will be available for periodic subscriptions.</t>
+  </si>
+  <si>
+    <t>As an administrator I will update Target consumption period(monthly,quarterly,half yearly,yearly), target sale quantity(example: 5000 units per quarter etc) per consumption period, minimum profit margin(percentage), maximum profit margin, Demand to supply ratio, consumption frequency(units per month)  for the registered item to register it as a subscriptionable item.</t>
+  </si>
+  <si>
+    <t>As a administrator I will "add" a new configuration paramter as Target Consumption period and its value with unit(1 month,1 yearetc)</t>
+  </si>
+  <si>
+    <t>As an administrator I will "add" a new configuration paramter "target sale per consumption period"and its value and unit.</t>
+  </si>
+  <si>
+    <t>As an administrator I will "add" a new configuration paramter "minimum profit margin", its value and unit.</t>
+  </si>
+  <si>
+    <t>As an administrator I will "add" a  new configuration parameter "maximum profit margin",its value and unit.</t>
+  </si>
+  <si>
+    <t>As an administrator I will "add" a  new configuration parameter "demand to supply ratio",its value and unit.</t>
+  </si>
+  <si>
+    <t>As an administrator I will "add" a  new configuration parameter "consumption frequency",its value and unit.</t>
+  </si>
+  <si>
+    <t>Mass upload</t>
+  </si>
+  <si>
+    <t>As an administrator I can add a new subscription rule "minimum permissible discount",its value and unit for a subscriptionable item so that subscriber fitting into various offers criterias can get minimum this vaue as discount.</t>
+  </si>
+  <si>
+    <t>As an administrator I can define the maximum discount percentage permissible for a subscriptionable item(including the added discounts due to offers and rewards).</t>
+  </si>
+  <si>
+    <t>As an administrator I can add a new subscription rule "maximum permissible discount",its value and unit for a subscriptionable item so that subscriber fitting into various offers criterias can get upto this value as discount.</t>
+  </si>
+  <si>
+    <t>As an administrator I can define maximum units of a subscriptionable itemthose can be subscribed per subscription cycle</t>
+  </si>
+  <si>
+    <t>As an administrator I can add a new subscription rule "maximum permissible units",its value and unit for a subscriptionable item so that subscriber can order upto this value per subscripton cycle.</t>
+  </si>
+  <si>
+    <t>As an administrator I will add new rule  "maximum permissible subscription period ",it value and unit so that any item cannot be subscribed at a time for more than the given value.</t>
+  </si>
+  <si>
+    <t>As an administrator I will add a new rule for the subscription basket "maximum permissible amount of the basket", as value and unit(rupees,dollor,euro etc)</t>
+  </si>
+  <si>
+    <t>As an administrator I will add a new rule "minimum threshold amount of basket for discount eligiibiity", value and unit for which the basket may be elligible for basket level discount/offer.</t>
+  </si>
+  <si>
+    <t>As an administrator I will add a new rule "maximum permissible discount", unit and value so that any subscriber cannot get discount more than the one defined here .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a administrator I will configure "Benefit" after becoming eligible as per the above criteria, by entering following parameters
+1. Benefit Type (Amount , coupons,redeempton points) 
+2. Benefit Value
+3. Unit (unit,currency or percentage)
+4. Benefit after (Only applicable in case of 'cashback' benefit type) days
+</t>
+  </si>
+  <si>
+    <t>As a administrator I will create new offer strategy  "Discount on Subscription basket" and add one or more crierias using. 
+1. Eligibility  criteria Parameter
+     a. Total Amount
+     b. Subscription period
+2. Comparator (Less than, equal to, Less than equal to, Greater than, Greater than equal to)
+3. Value
+4. Unit
+So that I can set the thresholds which are applicable for being eiigible for basket level discount.</t>
   </si>
   <si>
     <t>As a administrator I will create new offer strategy where I will choose offer type as "Brand Loyalty Program" and selects the following
 1. Brand (Select from dropdown)
-2. Eligibility  criteria (Total Amount or Subscription period)
-3. Comparator (less that equal to or greater than equal to)
-4. Value type (time period or amount)
-5. Value
-6. Unit (currency or days)
-There can be multiple eligibility criterias. In that case, I as administrator will add those by selecting above parameters from 2 to 6 for each criteria.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a administrator I will configure benefit on offer by entering following parameters
-1. Benefit Type (Amount or percentage or cashback or coupon) 
-2. Benefit
-3. Unit of benefit (currency or percentage)
-4. Time period for cashback (Only applicable in case of 'cashback' benefit type)
+2. Eligibility  criteria Parameter
+     a. Total Amount
+     b. Subscription period
+3. Comparator (Less than, equal to, Less than equal to, Greater than, Greater than equal to)
+4. Value
+5. Unit
+So that I can set the thresholds which are applicable for being eiigible for basket level discount.</t>
+  </si>
+  <si>
+    <t>As a administrator I will create new offer strategy where I will choose offer type as "Customer Loyalty" and selects the following
+1. Eligibility  criteria Parameter
+     a. Total Amount
+     b. Subscription period
+2. Comparator (Less than, equal to, Less than equal to, Greater than, Greater than equal to)
+3. Value
+4. Unit
+So that I can set the thresholds which are applicable for being eiigible for basket level discount.</t>
+  </si>
+  <si>
+    <t>As a administrator I will create new offer strategy where I will choose Start Date, End Date and Offer Type as "Surprise Offer" and selects the following
+1. Eligibility  criteria Parameter
+     a. Total Amount
+     b. Subscription period
+2. Comparator (Less than, equal to, Less than equal to, Greater than, Greater than equal to)
+3. Value
+4. Unit
+So that I can set the thresholds which are applicable for being eiigible for basket level discount.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a administrator I will configure "Benefit" after becoming eligible as per the above criteria, by entering following parameters
+1. Benefit Type (Amount , coupons,redeempton points) 
+2. Benefit Value
+3. Unit (unit,currency or percentage)
+4. Benefit after (Only applicable in case of 'cashback' benefit type) days.
 </t>
-  </si>
-  <si>
-    <t>Create surprise offer</t>
-  </si>
-  <si>
-    <t>As a administrator I will create new offer strategy where I will choose Start Date, End Date and Offer Type as "Surprise Offer" and selects the following
-1. Eligibility  criteria (Total Amount or Subscription period)
-2. Comparator (less that equal to or greater than equal to)
-3. Value type (time period or amount)
-4. Value
-5. Unit (currency or days)
-There can be multiple eligibility criterias. In that case, I as administrator will add those by selecting above 5 parameters for each criteria.</t>
-  </si>
-  <si>
-    <t>Generate dispatch requests for the next day</t>
-  </si>
-  <si>
-    <t>As a system I will generate a file on a daily basis containing the subscriberId,list of products selected by him/her(category id,subcategory Id,item id,quoted price of each item subscribed under his basket) and intended delivery date  so as to make the dispatch department enable the actual dispatch of these items as well as consolidate if the required dispatch were made on that day or not.</t>
-  </si>
-  <si>
-    <t>System will receive the status(DISPATCH,DEIVERED,DELIVERY FAILED) with reason code  of raised dispatch requests,from dispatch/delivery departments in the form of a flat file so as to update the same in the repository .</t>
-  </si>
-  <si>
-    <t>Daily retrival of subscriptionable items datails from main store.</t>
-  </si>
-  <si>
-    <t>During transition of one batch of product to new batch the purchase price may change.</t>
-  </si>
-  <si>
-    <t>As a system I will retrieve the BatchID,Category(CategoryId,Category Name), subcategory(subcategory id and subcategory name),Item under each category/subcategory only those which are registered as subscriptionable item,its latest purchase price,its current stock,its current MRP and its current quoted price(for instantanious sale) on a daily basis so as to maintain/update the inventory proxy.</t>
-  </si>
-  <si>
-    <t>Should I forecast for the probable increase of demand in the remaining days of month.</t>
-  </si>
-  <si>
-    <t>As a system I will generate a flat file containing category,subcategory, subscriptionable item id and its current stock requirement (as of the day) and increment in the stock as compared to earlier day which can be considered as a forecast of next three months for the inventory department.</t>
-  </si>
-  <si>
-    <t>As an Administrator I will retrieve the list of available items from current inventory of shopping application,optionally by providing category and subcategory as a search criteria so as to register them to be subcriptionable item.</t>
-  </si>
-  <si>
-    <t>As an administrator I will select an item to be register as a subscriptionable item and register it with system so that only these items will be available for periodic subscriptions.</t>
-  </si>
-  <si>
-    <t>As an administrator I will update Target consumption period(monthly,quarterly,half yearly,yearly), target sale quantity(example: 5000 units per quarter etc) per consumption period, minimum profit margin(percentage), maximum profit margin, Demand to supply ratio, consumption frequency(units per month)  for the registered item to register it as a subscriptionable item.</t>
-  </si>
-  <si>
-    <t>As a administrator I will "add" a new configuration paramter as Target Consumption period and its value with unit(1 month,1 yearetc)</t>
-  </si>
-  <si>
-    <t>As an administrator I will "add" a new configuration paramter "target sale per consumption period"and its value and unit.</t>
-  </si>
-  <si>
-    <t>As an administrator I will "add" a new configuration paramter "minimum profit margin", its value and unit.</t>
-  </si>
-  <si>
-    <t>As an administrator I will "add" a  new configuration parameter "maximum profit margin",its value and unit.</t>
-  </si>
-  <si>
-    <t>As an administrator I will "add" a  new configuration parameter "demand to supply ratio",its value and unit.</t>
-  </si>
-  <si>
-    <t>As an administrator I will "add" a  new configuration parameter "consumption frequency",its value and unit.</t>
-  </si>
-  <si>
-    <t>Mass upload</t>
-  </si>
-  <si>
-    <t>As an administrator I can add a new subscription rule "minimum permissible discount",its value and unit for a subscriptionable item so that subscriber fitting into various offers criterias can get minimum this vaue as discount.</t>
-  </si>
-  <si>
-    <t>As an administrator I can define the maximum discount percentage permissible for a subscriptionable item(including the added discounts due to offers and rewards).</t>
-  </si>
-  <si>
-    <t>As an administrator I can add a new subscription rule "maximum permissible discount",its value and unit for a subscriptionable item so that subscriber fitting into various offers criterias can get upto this value as discount.</t>
-  </si>
-  <si>
-    <t>As an administrator I can define maximum units of a subscriptionable itemthose can be subscribed per subscription cycle</t>
-  </si>
-  <si>
-    <t>As an administrator I can add a new subscription rule "maximum permissible units",its value and unit for a subscriptionable item so that subscriber can order upto this value per subscripton cycle.</t>
-  </si>
-  <si>
-    <t>As an administrator I will add new rule  "maximum permissible subscription period ",it value and unit so that any item cannot be subscribed at a time for more than the given value.</t>
-  </si>
-  <si>
-    <t>As an administrator I will add a new rule for the subscription basket "maximum permissible amount of the basket", as value and unit(rupees,dollor,euro etc)</t>
-  </si>
-  <si>
-    <t>As an administrator I will add a new rule "minimum threshold amount of basket for discount eligiibiity", value and unit for which the basket may be elligible for basket level discount/offer.</t>
-  </si>
-  <si>
-    <t>As an administrator I will add a new rule "maximum permissible discount", unit and value so that any subscriber cannot get discount more than the one defined here .</t>
   </si>
 </sst>
 </file>
@@ -1012,66 +915,66 @@
   <sheetData>
     <row r="2" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C2" s="7" t="s">
-        <v>127</v>
+        <v>88</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>128</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
-        <v>113</v>
+        <v>74</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>123</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
-        <v>114</v>
+        <v>75</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>115</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
-        <v>116</v>
+        <v>77</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>117</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C6" s="6" t="s">
-        <v>118</v>
+        <v>79</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>119</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C7" s="6" t="s">
-        <v>121</v>
+        <v>82</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="6" t="s">
-        <v>122</v>
+        <v>83</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C9" s="6" t="s">
-        <v>125</v>
+        <v>86</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>126</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.25">
@@ -1454,1165 +1357,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H101"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.140625" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="69.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="83.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-    </row>
-    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-    </row>
-    <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-    </row>
-    <row r="39" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-      <c r="H39" s="1"/>
-    </row>
-    <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-    </row>
-    <row r="41" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1"/>
-    </row>
-    <row r="42" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-    </row>
-    <row r="43" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-    </row>
-    <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-    </row>
-    <row r="45" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
-      <c r="H46" s="1"/>
-    </row>
-    <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="D47" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
-      <c r="H47" s="1"/>
-    </row>
-    <row r="48" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="D48" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
-      <c r="H48" s="1"/>
-    </row>
-    <row r="49" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="D49" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
-      <c r="H49" s="1"/>
-    </row>
-    <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="D50" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1"/>
-    </row>
-    <row r="51" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="D51" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-    </row>
-    <row r="53" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-      <c r="F54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="1"/>
-      <c r="H55" s="1"/>
-    </row>
-    <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="1"/>
-      <c r="H56" s="1"/>
-    </row>
-    <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1"/>
-      <c r="H57" s="1"/>
-    </row>
-    <row r="58" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-    </row>
-    <row r="59" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="1"/>
-      <c r="H59" s="1"/>
-    </row>
-    <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="1"/>
-      <c r="H60" s="1"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1"/>
-      <c r="H61" s="1"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="1"/>
-      <c r="H62" s="1"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
-      <c r="G63" s="1"/>
-      <c r="H63" s="1"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="1"/>
-      <c r="H64" s="1"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
-      <c r="G65" s="1"/>
-      <c r="H65" s="1"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="1"/>
-      <c r="H66" s="1"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
-      <c r="B67" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="1"/>
-      <c r="H67" s="1"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
-      <c r="B68" s="1"/>
-      <c r="C68" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1"/>
-      <c r="H68" s="1"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
-      <c r="B69" s="1"/>
-      <c r="C69" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
-      <c r="B71" s="1"/>
-      <c r="C71" s="1"/>
-      <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
-      <c r="G71" s="1"/>
-      <c r="H71" s="1"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1"/>
-      <c r="H72" s="1"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
-      <c r="G73" s="1"/>
-      <c r="H73" s="1"/>
-    </row>
-    <row r="74" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
-      <c r="B74" s="1"/>
-      <c r="C74" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D74" s="1"/>
-      <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
-      <c r="G74" s="1"/>
-      <c r="H74" s="1"/>
-    </row>
-    <row r="75" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
-      <c r="B75" s="1"/>
-      <c r="C75" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D75" s="1"/>
-      <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
-      <c r="G75" s="1"/>
-      <c r="H75" s="1"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
-      <c r="B76" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D76" s="1"/>
-      <c r="E76" s="1"/>
-      <c r="F76" s="1"/>
-      <c r="G76" s="1"/>
-      <c r="H76" s="1"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
-      <c r="B77" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D77" s="1"/>
-      <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
-      <c r="G77" s="1"/>
-      <c r="H77" s="1"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D78" s="1"/>
-      <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
-      <c r="G78" s="1"/>
-      <c r="H78" s="1"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D79" s="1"/>
-      <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1"/>
-      <c r="H79" s="1"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
-      <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
-      <c r="H81" s="1"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
-      <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
-      <c r="H82" s="1"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="1"/>
-      <c r="D83" s="1"/>
-      <c r="E83" s="1"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
-      <c r="H83" s="1"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="1"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
-      <c r="G84" s="1"/>
-      <c r="H84" s="1"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="1"/>
-      <c r="D85" s="1"/>
-      <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
-      <c r="G85" s="1"/>
-      <c r="H85" s="1"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
-      <c r="G86" s="1"/>
-      <c r="H86" s="1"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="1"/>
-      <c r="D87" s="1"/>
-      <c r="E87" s="1"/>
-      <c r="F87" s="1"/>
-      <c r="G87" s="1"/>
-      <c r="H87" s="1"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
-      <c r="B88" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C88" s="1"/>
-      <c r="D88" s="1"/>
-      <c r="E88" s="1"/>
-      <c r="F88" s="1"/>
-      <c r="G88" s="1"/>
-      <c r="H88" s="1"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="1"/>
-      <c r="B89" s="1"/>
-      <c r="C89" s="1"/>
-      <c r="D89" s="1"/>
-      <c r="E89" s="1"/>
-      <c r="F89" s="1"/>
-      <c r="G89" s="1"/>
-      <c r="H89" s="1"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="1"/>
-      <c r="B90" s="1"/>
-      <c r="C90" s="1"/>
-      <c r="D90" s="1"/>
-      <c r="E90" s="1"/>
-      <c r="F90" s="1"/>
-      <c r="G90" s="1"/>
-      <c r="H90" s="1"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="1"/>
-      <c r="B91" s="1"/>
-      <c r="C91" s="1"/>
-      <c r="D91" s="1"/>
-      <c r="E91" s="1"/>
-      <c r="F91" s="1"/>
-      <c r="G91" s="1"/>
-      <c r="H91" s="1"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="1"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1"/>
-      <c r="E92" s="1"/>
-      <c r="F92" s="1"/>
-      <c r="G92" s="1"/>
-      <c r="H92" s="1"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="B93" s="1"/>
-      <c r="C93" s="1"/>
-      <c r="D93" s="1"/>
-      <c r="E93" s="1"/>
-      <c r="F93" s="1"/>
-      <c r="G93" s="1"/>
-      <c r="H93" s="1"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="1"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="1"/>
-      <c r="D94" s="1"/>
-      <c r="E94" s="1"/>
-      <c r="F94" s="1"/>
-      <c r="G94" s="1"/>
-      <c r="H94" s="1"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="1"/>
-      <c r="B95" s="1"/>
-      <c r="C95" s="1"/>
-      <c r="D95" s="1"/>
-      <c r="E95" s="1"/>
-      <c r="F95" s="1"/>
-      <c r="G95" s="1"/>
-      <c r="H95" s="1"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="1"/>
-      <c r="B96" s="1"/>
-      <c r="C96" s="1"/>
-      <c r="D96" s="1"/>
-      <c r="E96" s="1"/>
-      <c r="F96" s="1"/>
-      <c r="G96" s="1"/>
-      <c r="H96" s="1"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="1"/>
-      <c r="B97" s="1"/>
-      <c r="C97" s="1"/>
-      <c r="D97" s="1"/>
-      <c r="E97" s="1"/>
-      <c r="F97" s="1"/>
-      <c r="G97" s="1"/>
-      <c r="H97" s="1"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-      <c r="C98" s="1"/>
-      <c r="D98" s="1"/>
-      <c r="E98" s="1"/>
-      <c r="F98" s="1"/>
-      <c r="G98" s="1"/>
-      <c r="H98" s="1"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-      <c r="B99" s="1"/>
-      <c r="C99" s="1"/>
-      <c r="D99" s="1"/>
-      <c r="E99" s="1"/>
-      <c r="F99" s="1"/>
-      <c r="G99" s="1"/>
-      <c r="H99" s="1"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="1"/>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
-      <c r="E100" s="1"/>
-      <c r="F100" s="1"/>
-      <c r="G100" s="1"/>
-      <c r="H100" s="1"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
-      <c r="E101" s="1"/>
-      <c r="F101" s="1"/>
-      <c r="G101" s="1"/>
-      <c r="H101" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0"/>
+    <sheetView topLeftCell="A27" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="47.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2624,22 +1373,22 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
       <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1"/>
       <c r="E2" s="4"/>
@@ -2653,21 +1402,21 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>162</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>163</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>164</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2675,7 +1424,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="5" t="s">
-        <v>165</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -2683,46 +1432,46 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="5" t="s">
-        <v>166</v>
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="D8" s="5" t="s">
-        <v>167</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="D9" s="5" t="s">
-        <v>168</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="D10" s="5" t="s">
-        <v>169</v>
+        <v>126</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="D11" s="5" t="s">
-        <v>170</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>171</v>
+        <v>128</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="D12" s="5"/>
     </row>
@@ -2730,7 +1479,7 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="D13" s="5"/>
     </row>
@@ -2742,10 +1491,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>129</v>
+        <v>90</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>130</v>
+        <v>91</v>
       </c>
       <c r="C15" s="1"/>
     </row>
@@ -2754,60 +1503,60 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="5" t="s">
-        <v>172</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>173</v>
+        <v>130</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>174</v>
+        <v>131</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>175</v>
+        <v>132</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>176</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>177</v>
+        <v>134</v>
       </c>
       <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>178</v>
+        <v>135</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>179</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>180</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2815,42 +1564,42 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>85</v>
+        <v>46</v>
       </c>
       <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
-        <v>86</v>
+        <v>47</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>88</v>
+        <v>49</v>
       </c>
       <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="D27" s="8"/>
     </row>
     <row r="28" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="5"/>
@@ -2878,7 +1627,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I83"/>
   <sheetViews>
@@ -2897,13 +1646,13 @@
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -2919,46 +1668,46 @@
     </row>
     <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>157</v>
+        <v>114</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>159</v>
+        <v>116</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>158</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>132</v>
+        <v>93</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>161</v>
+        <v>118</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>160</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>154</v>
+        <v>111</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>155</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>156</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -3340,12 +2089,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:XFD26"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3359,13 +2108,13 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -3376,26 +2125,26 @@
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>145</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
-        <v>146</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -3403,130 +2152,130 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>130</v>
+        <v>91</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>94</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>96</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>95</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>110</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>139</v>
+        <v>100</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>140</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>141</v>
+        <v>102</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>134</v>
+        <v>95</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>133</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>137</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
-        <v>138</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="3" t="s">
-        <v>135</v>
+        <v>96</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>136</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3535,111 +2284,111 @@
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>111</v>
+        <v>72</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>98</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
-        <v>112</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
-        <v>99</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
-        <v>100</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1" t="s">
-        <v>101</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
-        <v>103</v>
+        <v>64</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>102</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="C35" s="1" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="C36" s="1" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="C37" s="1" t="s">
-        <v>104</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="C38" s="1" t="s">
-        <v>106</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="C39" s="1" t="s">
-        <v>105</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="C40" s="1" t="s">
-        <v>108</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>107</v>
+        <v>68</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="C42" s="1" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="C43" s="1" t="s">
-        <v>109</v>
+        <v>70</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -3649,10 +2398,10 @@
     <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -3667,38 +2416,38 @@
     </row>
     <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="C48" s="1"/>
     </row>
     <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="C49" s="1"/>
     </row>
     <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="C50" s="1"/>
     </row>
     <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="C51" s="1"/>
     </row>
     <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C52" s="1"/>
     </row>
@@ -3714,10 +2463,10 @@
     </row>
     <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="C55" s="1"/>
     </row>
@@ -3738,31 +2487,31 @@
     </row>
     <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="C59" s="1"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1" t="s">
-        <v>61</v>
+        <v>24</v>
       </c>
       <c r="C60" s="1"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="2" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="C61" s="1"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1" t="s">
-        <v>63</v>
+        <v>26</v>
       </c>
       <c r="C62" s="1"/>
     </row>
@@ -3781,7 +2530,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
@@ -3799,65 +2548,65 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>66</v>
+        <v>28</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>67</v>
+        <v>29</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>70</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>71</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>72</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -3903,7 +2652,7 @@
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>73</v>
+        <v>35</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -3938,12 +2687,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3956,78 +2705,78 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
-        <v>143</v>
+        <v>104</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="8" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>144</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>147</v>
+        <v>108</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="8" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>149</v>
+        <v>109</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="8" t="s">
-        <v>151</v>
+        <v>138</v>
       </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>152</v>
+        <v>110</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="8" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D9" s="3"/>
     </row>

</xml_diff>

<commit_message>
Updated user subscription user story
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.001.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.001.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\affaince\documentation\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\affaince\documentation\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="139">
   <si>
     <t>Epics</t>
   </si>
@@ -97,21 +97,6 @@
     <t>System suspends subscription order due to absence of payment</t>
   </si>
   <si>
-    <t>Cancelled Subscription</t>
-  </si>
-  <si>
-    <t>Subcriber unsubscribing from one or more subscribed items</t>
-  </si>
-  <si>
-    <t>Unregister a subscriber</t>
-  </si>
-  <si>
-    <t>System cancells subscription order after the grace perod of payment is over</t>
-  </si>
-  <si>
-    <t>System recovers maximum pending pament form the available deposit.</t>
-  </si>
-  <si>
     <t>Configure system for the price calculation options.</t>
   </si>
   <si>
@@ -145,16 +130,7 @@
     <t>Detailed User Stories</t>
   </si>
   <si>
-    <t>As an administrator I will configure the minimum thrshold amount of the basket for which the basket may be elligible for baset level discount.</t>
-  </si>
-  <si>
     <t>System will validate the received category information and Item information against the main application inventory as well as retrieve additional information such as category/sbcategory name,item name,manufacturer Id and Name,purchase price,MRP,current stock so as to list them on Configuration UI for the registration purpose.</t>
-  </si>
-  <si>
-    <t>As an Administrator I will create notification rule by configuring the minimum stock threshold of an item( number and unit(percentage,units)) below which a notification should be sent to inventory for urgently procuring that item from supplyer,manufacturer</t>
-  </si>
-  <si>
-    <t>As an Administrator I will retrieve the list of available items from current inventory of shopping application by providing category and subcategory as a search criteria so as to register them to be subcriptionable item.</t>
   </si>
   <si>
     <t>Periodic batch operations</t>
@@ -168,9 +144,6 @@
   </si>
   <si>
     <t>Update status of targeted dispatches on every day</t>
-  </si>
-  <si>
-    <t>As an administrator I will configure the rule for the subscription basket such that maximum permissible subscription period of any item in the basket should not exceed configured duration as number and unit(month, year).</t>
   </si>
   <si>
     <t>Configure Payment Modes</t>
@@ -219,20 +192,6 @@
 THis is how he is configuring the payment to be made for every subscripton cycle in advance.</t>
   </si>
   <si>
-    <t>As an administrator I can define the maximum discount percentage permissible for a subscriptionable item(including the added discounts due to offers and rewards)</t>
-  </si>
-  <si>
-    <t>As an administrator I can define the maximum discount percentage permissible for a subscription basket(including the added discounts due to offers and rewards).</t>
-  </si>
-  <si>
-    <t>As an administrator I will configure the rules for the subscription baskets such as maximum permissible amount of the basket per subscription cycle,as number and unit(rupees,dollor,euro etc)</t>
-  </si>
-  <si>
-    <t>As an administrator I can define maximum units those can be subscribed per subscription cycle as
-Units:
-subscription cycle:</t>
-  </si>
-  <si>
     <t>As a system I calculate current price quote for the the subscription item which the user is intending to subscribe and show it as today's offered price,MRP, perentage gain.</t>
   </si>
   <si>
@@ -269,15 +228,6 @@
     <t>As a system I will recalculate and display the revised prices of the items in the user's basket so as to accommodate the removal of subscriptionable items from the basket.</t>
   </si>
   <si>
-    <t>As an administrator I can configure the maximum number of subscription baskets a subscriber can have.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a User  I add a subscription item to a subscription basket by providing qunatity per cycle, so as to subscribe for that item.   </t>
-  </si>
-  <si>
-    <t>As a User I keep on adding subscription items to one of my created baskets so as to build my subscription basket and finally checkout the basket after finalizing subscription items so as to get the total price to be paid as well as total gain( as compared to total MRP).</t>
-  </si>
-  <si>
     <t>Subscription</t>
   </si>
   <si>
@@ -336,24 +286,6 @@
   </si>
   <si>
     <t>Generate stock of subscriptions on a day with quotes per item</t>
-  </si>
-  <si>
-    <t>As a system I will create a default subscription portfolio identified by the subscriber Id for every subscriber so that the subscriber can add one or more subscription baskets in it</t>
-  </si>
-  <si>
-    <t>Create defaults</t>
-  </si>
-  <si>
-    <t>Create new/additional subscription basket</t>
-  </si>
-  <si>
-    <t>As a user I create a new/additional subscription basket by providing name,subscription cycle in the form of  Number describing periodicity , and unit for it( 2 week,3 month etc.) , subscription period and payment mode.</t>
-  </si>
-  <si>
-    <t>As a System I will create a default subscription basket with id=subcriberId_Basket1  and default subscription cycle as one month and defaut subscription period as one year  and default payment mode as full advanced payment for the subscription period so that customer can use it for adding subscripionble items in it if he/she doesn't want to create multiple subscription baskets under his subsription portfolio</t>
-  </si>
-  <si>
-    <t>As a user I will modify the ID of the default subscription basket,subscription cycle,subscription period and payment mode</t>
   </si>
   <si>
     <t>Register as a subscriber</t>
@@ -373,12 +305,6 @@
   </si>
   <si>
     <t>TODO: In case of benefit type 'material', parameters need to finalize</t>
-  </si>
-  <si>
-    <t>As an administrator I will select an item to be register as a subscriptionable item and register it with system so that only registered items will be available for periodic subscriptions.</t>
-  </si>
-  <si>
-    <t>As an administrator I will update Target consumption period(monthly,quarterly,half yearly,yearly), target sale quantity(example: 5000 units per quarter etc).,minimum profit margin(percentage),maximum profit margin, Demand density(very high,high,medium,low,very low),Demand to supply ratio, consumption frequency(high,low,medium)  for the registered item to register as a subscriptionable item</t>
   </si>
   <si>
     <t>Create offer based on Brand Loyalty</t>
@@ -527,12 +453,69 @@
 4. Benefit after (Only applicable in case of 'cashback' benefit type) days.
 </t>
   </si>
+  <si>
+    <t xml:space="preserve">As a User  I add a subscription item to a subscription basket by providing subscryption cycle (weekly, monthly, twice a month, alternate months, quaterly), quantity per cycle and number of cycles, so as to subscribe for that item.   </t>
+  </si>
+  <si>
+    <t>As a User I keep on adding subscription items to basket by entering subscryption cycle (weekly, monthly, twice a month, alternate months, quaterly), quantity per cycle and number of cycles so as to build my subscription basket and finally checkout the basket after finalizing subscription items so as to get the total price to be paid as well as total gain( as compared to total MRP).</t>
+  </si>
+  <si>
+    <t>As a System I will run subscription item level validations and display error message in case of any validation fails.</t>
+  </si>
+  <si>
+    <t>As a System I will run basket level validations and display error message in case of any validation fails.</t>
+  </si>
+  <si>
+    <t>Revise Subscription</t>
+  </si>
+  <si>
+    <t>Add items into subscription basket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a User  I add a subscription item to a active subscription basket by providing subscryption cycle (weekly, monthly, twice a month, alternate months, quaterly), quantity per cycle and number of cycles, so as to subscribe for that item.   </t>
+  </si>
+  <si>
+    <t>As a system I will recalculate and show the revised price quotes for newly added subscription items based on the basket size/amount of basket,supply vs demand statistics of items selected etc.</t>
+  </si>
+  <si>
+    <t>As a System I display updated subscription basket containing list of intended subscription items'  payable price per item, total MRP per item,  percentage gain per item,total amout to be paid for the basket ,total MRP for the basket  and total savings in percentage  and in amount per basket per cycle.</t>
+  </si>
+  <si>
+    <t>System routes user to payment system. Payment system send event (success or failure) back to subscription system. Subscription system register revised subscription accordingly.</t>
+  </si>
+  <si>
+    <t>Unsubscribe items from subscription basket</t>
+  </si>
+  <si>
+    <t>As a user I can modify the quantity or number of cycle of one or more subscriptionable items from subscription basket screen.</t>
+  </si>
+  <si>
+    <t>As a user I can unsubscribe an already subscribed subscriptionable item from subscription basket screen.</t>
+  </si>
+  <si>
+    <t>As a system I will calculate refund amount and charges (Same as additional discount on delivered items provided to subscriber) and display on screen with 'Accept' and 'Cancel' buttons to take approval of user.</t>
+  </si>
+  <si>
+    <t>As a user I will accept calcellation in order to revise my subscription.</t>
+  </si>
+  <si>
+    <t>As a System I display updated subscription basket.</t>
+  </si>
+  <si>
+    <t>Cancel Subscription</t>
+  </si>
+  <si>
+    <t>User cancel subscription</t>
+  </si>
+  <si>
+    <t>As a user I will cancel subscription as to unsubscribe all items from subscription basket.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -550,6 +533,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -590,7 +580,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -617,6 +607,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -915,66 +908,66 @@
   <sheetData>
     <row r="2" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C2" s="7" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C3" s="6" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C6" s="6" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C7" s="6" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="3:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C8" s="6" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C9" s="6" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>87</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.25">
@@ -1376,10 +1369,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D1" s="4"/>
     </row>
@@ -1402,21 +1395,21 @@
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
-        <v>119</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
-        <v>120</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>121</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1424,7 +1417,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="5" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1432,46 +1425,46 @@
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="5" t="s">
-        <v>123</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="D8" s="5" t="s">
-        <v>124</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="D9" s="5" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="D10" s="5" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="D11" s="5" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="D12" s="5"/>
     </row>
@@ -1479,7 +1472,7 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D13" s="5"/>
     </row>
@@ -1491,10 +1484,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="C15" s="1"/>
     </row>
@@ -1503,60 +1496,60 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="5" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
       <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1564,42 +1557,42 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:5" ht="225" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="165" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D27" s="8"/>
     </row>
     <row r="28" spans="1:5" ht="150" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="5"/>
@@ -1649,10 +1642,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -1668,46 +1661,46 @@
     </row>
     <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>115</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -2093,8 +2086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2111,10 +2104,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
@@ -2124,356 +2117,366 @@
       <c r="I1" s="4"/>
     </row>
     <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="C4" s="1" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>40</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="B15" s="1"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
       <c r="C15" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="C19" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B18" s="1"/>
-      <c r="C18" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
     <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="C20" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="1" t="s">
-        <v>100</v>
-      </c>
       <c r="C21" s="1" t="s">
-        <v>101</v>
+        <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="1" t="s">
-        <v>95</v>
-      </c>
+      <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="3" t="s">
-        <v>96</v>
+      <c r="B26" s="1" t="s">
+        <v>12</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>97</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-    </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>72</v>
-      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="1"/>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="A29" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
+      <c r="B30" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C30" s="1"/>
     </row>
     <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1" t="s">
-        <v>60</v>
-      </c>
+      <c r="A31" s="10"/>
+      <c r="B31" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
+      <c r="B33" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="C35" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="C36" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="1"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="C37" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="C38" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="C39" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+    </row>
+    <row r="40" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>125</v>
+      </c>
       <c r="C40" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
-      <c r="C44" s="1"/>
-    </row>
-    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B44" s="1"/>
+      <c r="C44" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
-      <c r="B45" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="1"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="1"/>
+      <c r="C46" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
-      <c r="B47" s="2"/>
+      <c r="B47" s="1"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>14</v>
-      </c>
+    <row r="48" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
       <c r="B48" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C48" s="1"/>
-    </row>
-    <row r="49" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
-      <c r="B49" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C49" s="1"/>
+      <c r="B49" s="1"/>
+      <c r="C49" s="1" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="B50" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C50" s="1"/>
-    </row>
-    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B50" s="1"/>
+      <c r="C50" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
-      <c r="B51" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C51" s="1"/>
-    </row>
-    <row r="52" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
-      <c r="B52" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C52" s="1"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C52" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C55" s="1"/>
+      <c r="C55" s="5" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="1"/>
+      <c r="C56" s="1" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
@@ -2485,34 +2488,24 @@
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>23</v>
-      </c>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1"/>
+      <c r="B59" s="1"/>
       <c r="C59" s="1"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
-      <c r="B60" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="B60" s="1"/>
       <c r="C60" s="1"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
-      <c r="B61" s="2" t="s">
-        <v>25</v>
-      </c>
+      <c r="B61" s="2"/>
       <c r="C61" s="1"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
-      <c r="B62" s="1" t="s">
-        <v>26</v>
-      </c>
+      <c r="B62" s="1"/>
       <c r="C62" s="1"/>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
@@ -2551,62 +2544,62 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -2652,7 +2645,7 @@
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2708,75 +2701,75 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>
       <c r="C3" s="8" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>108</v>
+        <v>84</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="8" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>109</v>
+        <v>85</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B7" s="3"/>
       <c r="C7" s="8" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="B9" s="3"/>
       <c r="C9" s="8" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="D9" s="3"/>
     </row>

</xml_diff>

<commit_message>
Add Consumer Basket domain. Re-organize import in Axon-commons
</commit_message>
<xml_diff>
--- a/documentation/requirements/SubscriptionRequirements_v0.001.xlsx
+++ b/documentation/requirements/SubscriptionRequirements_v0.001.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\affaince\documentation\requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Applications\affaince\documentation\requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9740" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Terminologies used" sheetId="7" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="143">
   <si>
     <t>Epics</t>
   </si>
@@ -509,6 +509,18 @@
   </si>
   <si>
     <t>As a user I will cancel subscription as to unsubscribe all items from subscription basket.</t>
+  </si>
+  <si>
+    <t>Generate daily offered price for Subscriptionable item</t>
+  </si>
+  <si>
+    <t>As a system I will generate a file on a daily basis containing the itemId, productId, currentOfferedPrice as to provide daily offered price to shopping application.</t>
+  </si>
+  <si>
+    <t>As a system I will send event containing itemId, productId, currentOfferedPrice as to provide item's current offered price to itemregistration domain.</t>
+  </si>
+  <si>
+    <t>As a System I will calculate discount and current offered price as to give maximum discount to subscriber.</t>
   </si>
 </sst>
 </file>
@@ -898,15 +910,15 @@
       <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="5"/>
-    <col min="3" max="3" width="17.5703125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="102.42578125" style="5" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="5"/>
+    <col min="1" max="2" width="9.1796875" style="5"/>
+    <col min="3" max="3" width="17.54296875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="102.453125" style="5" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C2" s="7" t="s">
         <v>72</v>
       </c>
@@ -914,7 +926,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:4" ht="29" x14ac:dyDescent="0.35">
       <c r="C3" s="6" t="s">
         <v>58</v>
       </c>
@@ -922,7 +934,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:4" ht="29" x14ac:dyDescent="0.35">
       <c r="C4" s="6" t="s">
         <v>59</v>
       </c>
@@ -930,7 +942,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:4" ht="29" x14ac:dyDescent="0.35">
       <c r="C5" s="6" t="s">
         <v>61</v>
       </c>
@@ -938,7 +950,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C6" s="6" t="s">
         <v>63</v>
       </c>
@@ -946,7 +958,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:4" ht="29" x14ac:dyDescent="0.35">
       <c r="C7" s="6" t="s">
         <v>66</v>
       </c>
@@ -954,7 +966,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="3:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:4" ht="29" x14ac:dyDescent="0.35">
       <c r="C8" s="6" t="s">
         <v>67</v>
       </c>
@@ -962,7 +974,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C9" s="6" t="s">
         <v>70</v>
       </c>
@@ -970,375 +982,375 @@
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
     </row>
-    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
     </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
     </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C33" s="6"/>
       <c r="D33" s="6"/>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C35" s="6"/>
       <c r="D35" s="6"/>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C36" s="6"/>
       <c r="D36" s="6"/>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
     </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
     </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
     </row>
-    <row r="58" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
     </row>
-    <row r="59" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
     </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
     </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
     </row>
-    <row r="63" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
     </row>
-    <row r="64" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C64" s="6"/>
       <c r="D64" s="6"/>
     </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C65" s="6"/>
       <c r="D65" s="6"/>
     </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C66" s="6"/>
       <c r="D66" s="6"/>
     </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C67" s="6"/>
       <c r="D67" s="6"/>
     </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C68" s="6"/>
       <c r="D68" s="6"/>
     </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
     </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C70" s="6"/>
       <c r="D70" s="6"/>
     </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C71" s="6"/>
       <c r="D71" s="6"/>
     </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C72" s="6"/>
       <c r="D72" s="6"/>
     </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
     </row>
-    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
     </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
     </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
     </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
     </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
     </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C79" s="6"/>
       <c r="D79" s="6"/>
     </row>
-    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
     </row>
-    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C81" s="6"/>
       <c r="D81" s="6"/>
     </row>
-    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C82" s="6"/>
       <c r="D82" s="6"/>
     </row>
-    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="83" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C83" s="6"/>
       <c r="D83" s="6"/>
     </row>
-    <row r="84" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="84" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C84" s="6"/>
       <c r="D84" s="6"/>
     </row>
-    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="85" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C85" s="6"/>
       <c r="D85" s="6"/>
     </row>
-    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="86" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C86" s="6"/>
       <c r="D86" s="6"/>
     </row>
-    <row r="87" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="87" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C87" s="6"/>
       <c r="D87" s="6"/>
     </row>
-    <row r="88" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="88" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C88" s="6"/>
       <c r="D88" s="6"/>
     </row>
-    <row r="89" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C89" s="6"/>
       <c r="D89" s="6"/>
     </row>
-    <row r="90" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C90" s="6"/>
       <c r="D90" s="6"/>
     </row>
-    <row r="91" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C91" s="6"/>
       <c r="D91" s="6"/>
     </row>
-    <row r="92" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C92" s="6"/>
       <c r="D92" s="6"/>
     </row>
-    <row r="93" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C93" s="6"/>
       <c r="D93" s="6"/>
     </row>
-    <row r="94" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C94" s="6"/>
       <c r="D94" s="6"/>
     </row>
-    <row r="95" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="95" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C95" s="6"/>
       <c r="D95" s="6"/>
     </row>
-    <row r="96" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="96" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C96" s="6"/>
       <c r="D96" s="6"/>
     </row>
-    <row r="97" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C97" s="6"/>
       <c r="D97" s="6"/>
     </row>
-    <row r="98" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C98" s="6"/>
       <c r="D98" s="6"/>
     </row>
-    <row r="99" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C99" s="6"/>
       <c r="D99" s="6"/>
     </row>
-    <row r="100" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C100" s="6"/>
       <c r="D100" s="6"/>
     </row>
-    <row r="101" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C101" s="6"/>
       <c r="D101" s="6"/>
     </row>
-    <row r="102" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C102" s="6"/>
       <c r="D102" s="6"/>
     </row>
@@ -1352,19 +1364,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="47.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="47.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="47.7109375" style="3"/>
-    <col min="3" max="3" width="57.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="55.42578125" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="47.7109375" style="3"/>
+    <col min="1" max="2" width="47.7265625" style="3"/>
+    <col min="3" max="3" width="57.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="55.453125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="47.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1376,7 +1388,7 @@
       </c>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1391,28 +1403,28 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1420,7 +1432,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1428,35 +1440,35 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="D8" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="D9" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="D10" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="D11" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="101.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>104</v>
       </c>
@@ -1468,7 +1480,7 @@
       </c>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
@@ -1476,13 +1488,13 @@
       </c>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>74</v>
       </c>
@@ -1491,7 +1503,7 @@
       </c>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1499,7 +1511,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
@@ -1509,7 +1521,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
@@ -1519,7 +1531,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
@@ -1527,7 +1539,7 @@
       </c>
       <c r="D19" s="5"/>
     </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>76</v>
       </c>
@@ -1538,30 +1550,30 @@
         <v>111</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="159.5" x14ac:dyDescent="0.35">
       <c r="B25" s="5" t="s">
         <v>38</v>
       </c>
@@ -1570,7 +1582,7 @@
       </c>
       <c r="D25" s="5"/>
     </row>
-    <row r="26" spans="1:5" ht="225" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="217.5" x14ac:dyDescent="0.35">
       <c r="B26" s="3" t="s">
         <v>39</v>
       </c>
@@ -1578,7 +1590,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="165" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="B27" s="3" t="s">
         <v>42</v>
       </c>
@@ -1587,7 +1599,7 @@
       </c>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:5" ht="150" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="145" x14ac:dyDescent="0.35">
       <c r="B28" s="3" t="s">
         <v>44</v>
       </c>
@@ -1597,22 +1609,22 @@
       <c r="D28" s="8"/>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D30" s="8"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D31" s="8"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="D32" s="8"/>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D33" s="8"/>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D34" s="8"/>
     </row>
   </sheetData>
@@ -1624,20 +1636,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" style="3" customWidth="1"/>
-    <col min="2" max="2" width="57.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="57.54296875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="79" style="3" customWidth="1"/>
-    <col min="4" max="4" width="79.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="3"/>
+    <col min="4" max="4" width="79.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1654,12 +1666,12 @@
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -1673,7 +1685,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>77</v>
@@ -1685,7 +1697,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>87</v>
@@ -1694,7 +1706,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>36</v>
@@ -1703,375 +1715,383 @@
         <v>89</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="2"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A52" s="1"/>
       <c r="B52" s="2"/>
       <c r="C52" s="1"/>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2086,20 +2106,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="69.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="97.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="14.453125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="69.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="97.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2116,7 +2136,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
     </row>
-    <row r="3" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2124,7 +2144,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>78</v>
@@ -2133,7 +2153,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
@@ -2143,10 +2163,10 @@
         <v>80</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>7</v>
@@ -2155,7 +2175,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>8</v>
@@ -2164,97 +2184,97 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="C15" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="C16" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="C17" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="C18" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="C19" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="C20" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="C21" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="C22" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
@@ -2264,17 +2284,17 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="C24" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>12</v>
@@ -2283,17 +2303,17 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
         <v>14</v>
       </c>
@@ -2302,45 +2322,45 @@
       </c>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="10"/>
       <c r="B30" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="10"/>
       <c r="B31" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="10"/>
       <c r="B32" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="10"/>
       <c r="B33" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>20</v>
       </c>
@@ -2349,22 +2369,22 @@
       </c>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>124</v>
       </c>
@@ -2375,54 +2395,54 @@
         <v>126</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A48" s="1"/>
       <c r="B48" s="1" t="s">
         <v>130</v>
@@ -2431,33 +2451,33 @@
         <v>131</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C52" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>136</v>
       </c>
@@ -2468,52 +2488,52 @@
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="C55" s="5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C56" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" s="1"/>
       <c r="B57" s="2"/>
       <c r="C57" s="1"/>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A61" s="1"/>
       <c r="B61" s="2"/>
       <c r="C61" s="1"/>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -2531,15 +2551,15 @@
       <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="49.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="9.1796875" style="3"/>
+    <col min="2" max="2" width="49.54296875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="19.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2550,28 +2570,28 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -2580,7 +2600,7 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
@@ -2589,88 +2609,88 @@
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2688,15 +2708,15 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" customWidth="1"/>
-    <col min="3" max="3" width="97.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.5703125" customWidth="1"/>
+    <col min="1" max="1" width="38.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7265625" customWidth="1"/>
+    <col min="3" max="3" width="97.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2707,7 +2727,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
       <c r="B2" s="3" t="s">
         <v>82</v>
       </c>
@@ -2716,7 +2736,7 @@
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="B3" s="3"/>
       <c r="C3" s="8" t="s">
         <v>114</v>
@@ -2725,7 +2745,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="145" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
         <v>84</v>
       </c>
@@ -2734,14 +2754,14 @@
       </c>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
       <c r="C5" s="8" t="s">
         <v>114</v>
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>85</v>
       </c>
@@ -2750,14 +2770,14 @@
       </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="B7" s="3"/>
       <c r="C7" s="8" t="s">
         <v>114</v>
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="130.5" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
         <v>86</v>
       </c>
@@ -2766,7 +2786,7 @@
       </c>
       <c r="D8" s="3"/>
     </row>
-    <row r="9" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="101.5" x14ac:dyDescent="0.35">
       <c r="B9" s="3"/>
       <c r="C9" s="8" t="s">
         <v>119</v>

</xml_diff>